<commit_message>
added more items to eliminate list
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/src/test/resources/ExcelData/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="225">
   <si>
     <t>Diabetes</t>
   </si>
@@ -450,6 +450,9 @@
     <t xml:space="preserve"> pastries</t>
   </si>
   <si>
+    <t>mawa</t>
+  </si>
+  <si>
     <t>Garlic</t>
   </si>
   <si>
@@ -679,6 +682,15 @@
   </si>
   <si>
     <t>Frozen</t>
+  </si>
+  <si>
+    <t>whip</t>
+  </si>
+  <si>
+    <t>yoghurt</t>
+  </si>
+  <si>
+    <t>cream</t>
   </si>
 </sst>
 </file>
@@ -2016,10 +2028,12 @@
       <c r="C23" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="12" t="s">
+        <v>144</v>
+      </c>
       <c r="E23" s="12"/>
       <c r="F23" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>111</v>
@@ -2046,7 +2060,7 @@
     </row>
     <row r="24" ht="24.0" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>112</v>
@@ -2057,10 +2071,10 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -2084,10 +2098,10 @@
     </row>
     <row r="25" ht="24.0" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>38</v>
@@ -2095,10 +2109,10 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -2122,10 +2136,10 @@
     </row>
     <row r="26" ht="46.5" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>70</v>
@@ -2133,10 +2147,10 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -2160,10 +2174,10 @@
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>63</v>
@@ -2174,7 +2188,7 @@
         <v>31</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -2198,13 +2212,13 @@
     </row>
     <row r="28" ht="24.0" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
@@ -2212,7 +2226,7 @@
         <v>110</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -2236,21 +2250,21 @@
     </row>
     <row r="29" ht="35.25" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -2274,10 +2288,10 @@
     </row>
     <row r="30" ht="24.0" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="11"/>
@@ -2286,7 +2300,7 @@
         <v>132</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2310,7 +2324,7 @@
     </row>
     <row r="31" ht="35.25" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="8"/>
@@ -2320,7 +2334,7 @@
         <v>142</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -2344,14 +2358,14 @@
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2376,7 +2390,7 @@
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -2408,7 +2422,7 @@
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -2472,7 +2486,7 @@
     </row>
     <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -2511,7 +2525,7 @@
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -2536,14 +2550,14 @@
     </row>
     <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -2575,7 +2589,7 @@
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -2600,14 +2614,14 @@
     </row>
     <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -2632,14 +2646,14 @@
     </row>
     <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -2671,7 +2685,7 @@
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="12" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -2696,7 +2710,7 @@
     </row>
     <row r="43" ht="13.5" customHeight="1">
       <c r="A43" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -2726,7 +2740,7 @@
     </row>
     <row r="44" ht="13.5" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -2756,7 +2770,7 @@
     </row>
     <row r="45" ht="13.5" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -2786,7 +2800,7 @@
     </row>
     <row r="46" ht="13.5" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -2816,7 +2830,7 @@
     </row>
     <row r="47" ht="13.5" customHeight="1">
       <c r="A47" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -2846,7 +2860,7 @@
     </row>
     <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -2876,7 +2890,7 @@
     </row>
     <row r="49" ht="13.5" customHeight="1">
       <c r="A49" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -2906,7 +2920,7 @@
     </row>
     <row r="50" ht="13.5" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -2936,7 +2950,7 @@
     </row>
     <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -2966,7 +2980,7 @@
     </row>
     <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -2996,7 +3010,7 @@
     </row>
     <row r="53" ht="13.5" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -3026,7 +3040,7 @@
     </row>
     <row r="54" ht="13.5" customHeight="1">
       <c r="A54" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -3056,7 +3070,7 @@
     </row>
     <row r="55" ht="13.5" customHeight="1">
       <c r="A55" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
@@ -3086,7 +3100,7 @@
     </row>
     <row r="56" ht="13.5" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -3116,7 +3130,7 @@
     </row>
     <row r="57" ht="13.5" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
@@ -3146,7 +3160,7 @@
     </row>
     <row r="58" ht="13.5" customHeight="1">
       <c r="A58" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -3176,7 +3190,7 @@
     </row>
     <row r="59" ht="13.5" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -3206,7 +3220,7 @@
     </row>
     <row r="60" ht="13.5" customHeight="1">
       <c r="A60" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -3296,7 +3310,7 @@
     </row>
     <row r="63" ht="13.5" customHeight="1">
       <c r="A63" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -3326,7 +3340,7 @@
     </row>
     <row r="64" ht="13.5" customHeight="1">
       <c r="A64" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -3386,7 +3400,7 @@
     </row>
     <row r="66" ht="13.5" customHeight="1">
       <c r="A66" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -3416,7 +3430,7 @@
     </row>
     <row r="67" ht="13.5" customHeight="1">
       <c r="A67" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -3446,7 +3460,7 @@
     </row>
     <row r="68" ht="13.5" customHeight="1">
       <c r="A68" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
@@ -3476,7 +3490,7 @@
     </row>
     <row r="69" ht="13.5" customHeight="1">
       <c r="A69" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -3506,7 +3520,7 @@
     </row>
     <row r="70" ht="13.5" customHeight="1">
       <c r="A70" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -3536,7 +3550,7 @@
     </row>
     <row r="71" ht="13.5" customHeight="1">
       <c r="A71" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
@@ -3596,7 +3610,7 @@
     </row>
     <row r="73" ht="13.5" customHeight="1">
       <c r="A73" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
@@ -3656,7 +3670,7 @@
     </row>
     <row r="75" ht="13.5" customHeight="1">
       <c r="A75" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B75" s="11"/>
       <c r="C75" s="11"/>
@@ -3686,7 +3700,7 @@
     </row>
     <row r="76" ht="13.5" customHeight="1">
       <c r="A76" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -3716,7 +3730,7 @@
     </row>
     <row r="77" ht="13.5" customHeight="1">
       <c r="A77" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -3746,7 +3760,7 @@
     </row>
     <row r="78" ht="13.5" customHeight="1">
       <c r="A78" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
@@ -3776,7 +3790,7 @@
     </row>
     <row r="79" ht="13.5" customHeight="1">
       <c r="A79" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -3806,7 +3820,7 @@
     </row>
     <row r="80" ht="13.5" customHeight="1">
       <c r="A80" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -3836,7 +3850,7 @@
     </row>
     <row r="81" ht="13.5" customHeight="1">
       <c r="A81" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
@@ -3866,7 +3880,7 @@
     </row>
     <row r="82" ht="13.5" customHeight="1">
       <c r="A82" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
@@ -3896,7 +3910,7 @@
     </row>
     <row r="83" ht="13.5" customHeight="1">
       <c r="A83" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
@@ -3926,7 +3940,7 @@
     </row>
     <row r="84" ht="13.5" customHeight="1">
       <c r="A84" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="11"/>
@@ -3956,7 +3970,7 @@
     </row>
     <row r="85" ht="13.5" customHeight="1">
       <c r="A85" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="11"/>
@@ -4016,7 +4030,7 @@
     </row>
     <row r="87" ht="13.5" customHeight="1">
       <c r="A87" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="11"/>
@@ -4045,7 +4059,9 @@
       <c r="Z87" s="4"/>
     </row>
     <row r="88" ht="13.5" customHeight="1">
-      <c r="A88" s="11"/>
+      <c r="A88" s="12" t="s">
+        <v>222</v>
+      </c>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
@@ -4073,7 +4089,9 @@
       <c r="Z88" s="4"/>
     </row>
     <row r="89" ht="13.5" customHeight="1">
-      <c r="A89" s="11"/>
+      <c r="A89" s="12" t="s">
+        <v>223</v>
+      </c>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
@@ -4101,7 +4119,9 @@
       <c r="Z89" s="4"/>
     </row>
     <row r="90" ht="13.5" customHeight="1">
-      <c r="A90" s="11"/>
+      <c r="A90" s="12" t="s">
+        <v>224</v>
+      </c>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -4129,7 +4149,9 @@
       <c r="Z90" s="4"/>
     </row>
     <row r="91" ht="13.5" customHeight="1">
-      <c r="A91" s="11"/>
+      <c r="A91" s="12" t="s">
+        <v>144</v>
+      </c>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>

</xml_diff>